<commit_message>
update 'threads' up to 64
</commit_message>
<xml_diff>
--- a/results/Threaded_Pi_Calc.xlsx
+++ b/results/Threaded_Pi_Calc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Github\TheadedPiCalc\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D110DC-7665-469B-97DE-10B351CAE676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE57168-207D-4E3C-83C5-3FAD39AFC22B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{BEF189AD-A55E-4A15-AD1C-D8BCD278AFF7}"/>
   </bookViews>
@@ -207,10 +207,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Threaded_Pi_Calc!$B$1:$G$1</c:f>
+              <c:f>Threaded_Pi_Calc!$B$1:$I$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -228,33 +228,45 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Threaded_Pi_Calc!$B$2:$G$2</c:f>
+              <c:f>Threaded_Pi_Calc!$B$2:$I$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.28859699999999999</c:v>
+                  <c:v>0.397928</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14303299999999999</c:v>
+                  <c:v>0.200374</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.7018799999999993E-2</c:v>
+                  <c:v>9.8641000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3011099999999998E-2</c:v>
+                  <c:v>6.2548999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.50097E-2</c:v>
+                  <c:v>5.3941000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.5010300000000003E-2</c:v>
+                  <c:v>5.1896999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.8013E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.2322E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -306,10 +318,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Threaded_Pi_Calc!$B$1:$G$1</c:f>
+              <c:f>Threaded_Pi_Calc!$B$1:$I$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -327,33 +339,45 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Threaded_Pi_Calc!$B$3:$G$3</c:f>
+              <c:f>Threaded_Pi_Calc!$B$3:$I$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.39609800000000001</c:v>
+                  <c:v>0.39556999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19985900000000001</c:v>
+                  <c:v>0.200206</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.108024</c:v>
+                  <c:v>0.105281</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0013999999999998E-2</c:v>
+                  <c:v>5.6742000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.5010000000000001E-2</c:v>
+                  <c:v>4.2005000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.4010000000000001E-2</c:v>
+                  <c:v>4.4003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.2020000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2011E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1449,18 +1473,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF022D2E-3E35-470D-9E9B-C3B444AF1270}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="11" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>1</v>
       </c>
@@ -1479,51 +1504,69 @@
       <c r="G1">
         <v>16</v>
       </c>
+      <c r="H1">
+        <v>32</v>
+      </c>
+      <c r="I1">
+        <v>64</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.28859699999999999</v>
+        <v>0.397928</v>
       </c>
       <c r="C2">
-        <v>0.14303299999999999</v>
+        <v>0.200374</v>
       </c>
       <c r="D2">
-        <v>8.7018799999999993E-2</v>
+        <v>9.8641000000000006E-2</v>
       </c>
       <c r="E2">
-        <v>5.3011099999999998E-2</v>
+        <v>6.2548999999999993E-2</v>
       </c>
       <c r="F2">
-        <v>4.50097E-2</v>
+        <v>5.3941000000000003E-2</v>
       </c>
       <c r="G2">
-        <v>4.5010300000000003E-2</v>
+        <v>5.1896999999999999E-2</v>
+      </c>
+      <c r="H2">
+        <v>4.8013E-2</v>
+      </c>
+      <c r="I2">
+        <v>5.2322E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.39609800000000001</v>
+        <v>0.39556999999999998</v>
       </c>
       <c r="C3">
-        <v>0.19985900000000001</v>
+        <v>0.200206</v>
       </c>
       <c r="D3">
-        <v>0.108024</v>
+        <v>0.105281</v>
       </c>
       <c r="E3">
-        <v>6.0013999999999998E-2</v>
+        <v>5.6742000000000001E-2</v>
       </c>
       <c r="F3">
-        <v>4.5010000000000001E-2</v>
+        <v>4.2005000000000001E-2</v>
       </c>
       <c r="G3">
-        <v>4.4010000000000001E-2</v>
+        <v>4.4003E-2</v>
+      </c>
+      <c r="H3">
+        <v>4.2020000000000002E-2</v>
+      </c>
+      <c r="I3">
+        <v>4.2011E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>